<commit_message>
update to variable-keywords-table with zacat variable groups from EB/44.2bis(1996) and other fixes
</commit_message>
<xml_diff>
--- a/data-raw/eb_waves_filenames.xlsx
+++ b/data-raw/eb_waves_filenames.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkolc\Google Drive\Work in progress\eurobarometer\not_included\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkolc\Google Drive\Work in progress\eurobarometer\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F3A7B6-7922-4AED-9E16-C12BB6309012}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45DB8AD0-3029-421A-8E70-8D5AB49054BD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{22F6F60A-BAD7-471D-BDDB-2D550D00C391}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="158">
   <si>
     <t>ZA7579: Eurobarometer 92.1 (2019): Expectations and concerns of connected and automated driving, Attitudes of Europeans towards Air Quality, and Undeclared work in the European Union</t>
   </si>
@@ -501,6 +501,9 @@
   </si>
   <si>
     <t>ZA3086: Eurobarometer 50.1: Information Society Services, Food Quality, the Family, and Aid to Development November-December 1998</t>
+  </si>
+  <si>
+    <t>ZA5481: Eurobarometer 75.3 (May 2011) Europe 2020, Financial and Economic Crisis, European Union Budget, and the Common Agricultural Policy</t>
   </si>
 </sst>
 </file>
@@ -852,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A77350EC-0646-4F9C-B6EA-17C391BB966D}">
-  <dimension ref="A1:A157"/>
+  <dimension ref="A1:A158"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A157"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1182,470 +1185,476 @@
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>106</v>
+        <v>157</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>52</v>
+        <v>111</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>112</v>
+        <v>57</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>113</v>
+        <v>63</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>64</v>
+        <v>113</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>114</v>
+        <v>64</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>65</v>
+        <v>114</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>128</v>
+        <v>65</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>66</v>
+        <v>128</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>80</v>
+        <v>129</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>81</v>
+        <v>130</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>82</v>
+        <v>140</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>141</v>
+        <v>93</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>115</v>
+        <v>156</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
         <v>127</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>